<commit_message>
WIP 1.2.0 : laser done
</commit_message>
<xml_diff>
--- a/excel_import/laser_report_template.xlsx
+++ b/excel_import/laser_report_template.xlsx
@@ -5,22 +5,35 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://johnsonoutdoorsinc-my.sharepoint.com/personal/david_zhang_johnsonoutdoors_com/Documents/David's Stuff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://johnsonoutdoorsinc-my.sharepoint.com/personal/david_zhang_johnsonoutdoors_com/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="204" documentId="13_ncr:1_{A1CECE6E-458F-422C-A05E-4186ECEC6448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6C99763-AF86-4C5D-AD1B-E6F58EE287C9}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="13_ncr:1_{A1CECE6E-458F-422C-A05E-4186ECEC6448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59B32068-6EDB-49E9-BD34-E632D9E09F73}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Part Number :</t>
   </si>
@@ -31,12 +44,6 @@
     <t>Part Number</t>
   </si>
   <si>
-    <t>Serial Number</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
     <t>Date Created</t>
   </si>
   <si>
@@ -52,15 +59,6 @@
     <t>Laser Result Report</t>
   </si>
   <si>
-    <t>Data Matrix</t>
-  </si>
-  <si>
-    <t>Label ID</t>
-  </si>
-  <si>
-    <t>Defect Desc.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Generated Date : </t>
   </si>
   <si>
@@ -68,6 +66,18 @@
   </si>
   <si>
     <t>Created By</t>
+  </si>
+  <si>
+    <t>Product S/N</t>
+  </si>
+  <si>
+    <t>PCBA S/N</t>
+  </si>
+  <si>
+    <t>Device ID</t>
+  </si>
+  <si>
+    <t>WO No.</t>
   </si>
 </sst>
 </file>
@@ -216,6 +226,9 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -224,9 +237,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -545,10 +555,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -556,17 +566,16 @@
     <col min="1" max="1" width="5.140625" style="7" customWidth="1"/>
     <col min="2" max="3" width="22.42578125" style="7" customWidth="1"/>
     <col min="4" max="4" width="18.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="6" customWidth="1"/>
     <col min="6" max="6" width="15.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" style="18" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="8"/>
+    <col min="7" max="7" width="14.7109375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" style="6" customWidth="1"/>
+    <col min="9" max="9" width="25.28515625" style="18" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="8" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="1" customFormat="1" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" s="1" customFormat="1" ht="9.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="4"/>
       <c r="C1" s="8"/>
       <c r="D1" s="4"/>
@@ -574,37 +583,34 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="5"/>
-    </row>
-    <row r="2" spans="2:10" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="21"/>
-    </row>
-    <row r="3" spans="2:10" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" spans="2:9" s="1" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
+    </row>
+    <row r="3" spans="2:9" s="7" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="12"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="2:10" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="2:9" s="1" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="3"/>
@@ -612,10 +618,9 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="2:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="2:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>0</v>
       </c>
@@ -624,12 +629,12 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-      <c r="I5" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="12"/>
-    </row>
-    <row r="6" spans="2:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="2:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
         <v>1</v>
       </c>
@@ -638,12 +643,12 @@
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="I6" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" s="22"/>
-    </row>
-    <row r="7" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="2:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
@@ -651,56 +656,52 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="2:10" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="2:9" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="67" orientation="landscape" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>